<commit_message>
Fixed the issues with fails
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -252,10 +252,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="justify" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -264,8 +270,52 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="justify" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="justify" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="justify" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -273,32 +323,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="justify" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="justify" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="justify" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="justify" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" textRotation="90" wrapText="1"/>
@@ -309,40 +338,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="justify" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="justify" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="justify" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2663,7 +2663,7 @@
   <dimension ref="A1:Z82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -2696,28 +2696,28 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="44" t="inlineStr">
+      <c r="A1" s="42" t="inlineStr">
         <is>
           <t>Appendix "D"</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="44" t="inlineStr">
+      <c r="A2" s="42" t="inlineStr">
         <is>
           <t xml:space="preserve">( Refers to para - 17 (c) (i) </t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="45" t="inlineStr">
+      <c r="A3" s="43" t="inlineStr">
         <is>
           <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                 Wing : Army </t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="46" t="inlineStr">
+      <c r="A4" s="31" t="inlineStr">
         <is>
           <t>NOMINAL ROLL CUM RESULT SHEET - CERTIFICATE "A" EXAM 2019-2020</t>
         </is>
@@ -2729,8 +2729,8 @@
           <t xml:space="preserve">NAME OF UNIT                 :  7 CG BN NCC, BILASPUR (CG) </t>
         </is>
       </c>
-      <c r="E5" s="51" t="n"/>
-      <c r="T5" s="29" t="inlineStr">
+      <c r="E5" s="30" t="n"/>
+      <c r="T5" s="44" t="inlineStr">
         <is>
           <t xml:space="preserve">Held at :- BILASPUR (CG)  </t>
         </is>
@@ -2742,13 +2742,13 @@
           <t xml:space="preserve">NAME OF GROUP HQS  :  RAIPUR  (CG) </t>
         </is>
       </c>
-      <c r="E6" s="51" t="n"/>
-      <c r="T6" s="29" t="inlineStr">
+      <c r="E6" s="30" t="n"/>
+      <c r="T6" s="44" t="inlineStr">
         <is>
           <t>Held on :- 09/02/2020</t>
         </is>
       </c>
-      <c r="Z6" s="52" t="n"/>
+      <c r="Z6" s="29" t="n"/>
     </row>
     <row r="7" ht="5.25" customHeight="1" s="28">
       <c r="A7" t="inlineStr">
@@ -2756,216 +2756,216 @@
           <t xml:space="preserve">NAME OF DTE                   :  MP &amp; CG BHOPAL </t>
         </is>
       </c>
-      <c r="E7" s="51" t="n"/>
-      <c r="T7" s="29" t="n"/>
-      <c r="U7" s="29" t="n"/>
-      <c r="V7" s="29" t="n"/>
-      <c r="W7" s="29" t="n"/>
-      <c r="X7" s="29" t="n"/>
-      <c r="Y7" s="29" t="n"/>
+      <c r="E7" s="30" t="n"/>
+      <c r="T7" s="44" t="n"/>
+      <c r="U7" s="44" t="n"/>
+      <c r="V7" s="44" t="n"/>
+      <c r="W7" s="44" t="n"/>
+      <c r="X7" s="44" t="n"/>
+      <c r="Y7" s="44" t="n"/>
     </row>
     <row r="8" ht="53.25" customHeight="1" s="28">
-      <c r="A8" s="30" t="inlineStr">
+      <c r="A8" s="45" t="inlineStr">
         <is>
           <t>S. No.</t>
         </is>
       </c>
-      <c r="B8" s="33" t="inlineStr">
+      <c r="B8" s="46" t="inlineStr">
         <is>
           <t>Regimental CBSE Roll No.</t>
         </is>
       </c>
-      <c r="C8" s="34" t="inlineStr">
+      <c r="C8" s="47" t="inlineStr">
         <is>
           <t>Rank</t>
         </is>
       </c>
-      <c r="D8" s="33" t="inlineStr">
+      <c r="D8" s="46" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="E8" s="33" t="inlineStr">
+      <c r="E8" s="46" t="inlineStr">
         <is>
           <t>Father's Name</t>
         </is>
       </c>
-      <c r="F8" s="47" t="inlineStr">
+      <c r="F8" s="32" t="inlineStr">
         <is>
           <t>Date of Birth</t>
         </is>
       </c>
-      <c r="G8" s="43" t="inlineStr">
+      <c r="G8" s="52" t="inlineStr">
         <is>
           <t>Date of Enrollment</t>
         </is>
       </c>
-      <c r="H8" s="47" t="inlineStr">
+      <c r="H8" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">Date of Discharge  </t>
         </is>
       </c>
-      <c r="I8" s="47" t="inlineStr">
+      <c r="I8" s="32" t="inlineStr">
         <is>
           <t>Details of Camp Attended</t>
         </is>
       </c>
-      <c r="J8" s="35" t="inlineStr">
+      <c r="J8" s="39" t="inlineStr">
         <is>
           <t>Parade Attendance %</t>
         </is>
       </c>
-      <c r="K8" s="42" t="n"/>
-      <c r="L8" s="50" t="inlineStr">
+      <c r="K8" s="37" t="n"/>
+      <c r="L8" s="40" t="inlineStr">
         <is>
           <t xml:space="preserve">MARKS OBTAINED </t>
         </is>
       </c>
-      <c r="M8" s="40" t="n"/>
-      <c r="N8" s="40" t="n"/>
-      <c r="O8" s="40" t="n"/>
-      <c r="P8" s="40" t="n"/>
-      <c r="Q8" s="40" t="n"/>
-      <c r="R8" s="40" t="n"/>
-      <c r="S8" s="40" t="n"/>
-      <c r="T8" s="40" t="n"/>
-      <c r="U8" s="42" t="n"/>
-      <c r="V8" s="36" t="inlineStr">
+      <c r="M8" s="36" t="n"/>
+      <c r="N8" s="36" t="n"/>
+      <c r="O8" s="36" t="n"/>
+      <c r="P8" s="36" t="n"/>
+      <c r="Q8" s="36" t="n"/>
+      <c r="R8" s="36" t="n"/>
+      <c r="S8" s="36" t="n"/>
+      <c r="T8" s="36" t="n"/>
+      <c r="U8" s="37" t="n"/>
+      <c r="V8" s="41" t="inlineStr">
         <is>
           <t xml:space="preserve"> Total </t>
         </is>
       </c>
-      <c r="W8" s="35" t="inlineStr">
+      <c r="W8" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Bonus Marks </t>
         </is>
       </c>
-      <c r="X8" s="36" t="inlineStr">
+      <c r="X8" s="41" t="inlineStr">
         <is>
           <t xml:space="preserve">Final Grand Total </t>
         </is>
       </c>
-      <c r="Y8" s="35" t="inlineStr">
+      <c r="Y8" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Grading </t>
         </is>
       </c>
-      <c r="Z8" s="49" t="inlineStr">
+      <c r="Z8" s="38" t="inlineStr">
         <is>
           <t>Photo</t>
         </is>
       </c>
     </row>
     <row r="9" ht="36" customHeight="1" s="28">
-      <c r="A9" s="31" t="n"/>
-      <c r="B9" s="31" t="n"/>
-      <c r="C9" s="31" t="n"/>
-      <c r="D9" s="31" t="n"/>
-      <c r="E9" s="31" t="n"/>
-      <c r="F9" s="31" t="n"/>
-      <c r="G9" s="31" t="n"/>
-      <c r="H9" s="31" t="n"/>
-      <c r="I9" s="31" t="n"/>
-      <c r="J9" s="37" t="inlineStr">
+      <c r="A9" s="33" t="n"/>
+      <c r="B9" s="33" t="n"/>
+      <c r="C9" s="33" t="n"/>
+      <c r="D9" s="33" t="n"/>
+      <c r="E9" s="33" t="n"/>
+      <c r="F9" s="33" t="n"/>
+      <c r="G9" s="33" t="n"/>
+      <c r="H9" s="33" t="n"/>
+      <c r="I9" s="33" t="n"/>
+      <c r="J9" s="48" t="inlineStr">
         <is>
           <t>Year -I ,2014-15</t>
         </is>
       </c>
-      <c r="K9" s="38" t="inlineStr">
+      <c r="K9" s="49" t="inlineStr">
         <is>
           <t>Year II -,2015-16</t>
         </is>
       </c>
-      <c r="L9" s="39" t="inlineStr">
+      <c r="L9" s="50" t="inlineStr">
         <is>
           <t>Part -I : Drill</t>
         </is>
       </c>
-      <c r="M9" s="40" t="n"/>
-      <c r="N9" s="40" t="n"/>
-      <c r="O9" s="39" t="inlineStr">
+      <c r="M9" s="36" t="n"/>
+      <c r="N9" s="36" t="n"/>
+      <c r="O9" s="50" t="inlineStr">
         <is>
           <t>Part -II : WT</t>
         </is>
       </c>
-      <c r="P9" s="40" t="n"/>
-      <c r="Q9" s="40" t="n"/>
-      <c r="R9" s="41" t="inlineStr">
+      <c r="P9" s="36" t="n"/>
+      <c r="Q9" s="36" t="n"/>
+      <c r="R9" s="51" t="inlineStr">
         <is>
           <t>Part - III  Misc</t>
         </is>
       </c>
-      <c r="S9" s="41" t="inlineStr">
+      <c r="S9" s="51" t="inlineStr">
         <is>
           <t>Part -IV : Spl Subjencts</t>
         </is>
       </c>
-      <c r="T9" s="40" t="n"/>
-      <c r="U9" s="42" t="n"/>
-      <c r="V9" s="32" t="n"/>
-      <c r="W9" s="32" t="n"/>
-      <c r="X9" s="32" t="n"/>
-      <c r="Y9" s="32" t="n"/>
-      <c r="Z9" s="32" t="n"/>
+      <c r="T9" s="36" t="n"/>
+      <c r="U9" s="37" t="n"/>
+      <c r="V9" s="34" t="n"/>
+      <c r="W9" s="34" t="n"/>
+      <c r="X9" s="34" t="n"/>
+      <c r="Y9" s="34" t="n"/>
+      <c r="Z9" s="34" t="n"/>
     </row>
     <row r="10" ht="84.75" customHeight="1" s="28">
-      <c r="A10" s="32" t="n"/>
-      <c r="B10" s="32" t="n"/>
-      <c r="C10" s="32" t="n"/>
-      <c r="D10" s="32" t="n"/>
-      <c r="E10" s="32" t="n"/>
-      <c r="F10" s="32" t="n"/>
-      <c r="G10" s="32" t="n"/>
-      <c r="H10" s="32" t="n"/>
-      <c r="I10" s="32" t="n"/>
-      <c r="J10" s="32" t="n"/>
-      <c r="K10" s="32" t="n"/>
-      <c r="L10" s="35" t="inlineStr">
+      <c r="A10" s="34" t="n"/>
+      <c r="B10" s="34" t="n"/>
+      <c r="C10" s="34" t="n"/>
+      <c r="D10" s="34" t="n"/>
+      <c r="E10" s="34" t="n"/>
+      <c r="F10" s="34" t="n"/>
+      <c r="G10" s="34" t="n"/>
+      <c r="H10" s="34" t="n"/>
+      <c r="I10" s="34" t="n"/>
+      <c r="J10" s="34" t="n"/>
+      <c r="K10" s="34" t="n"/>
+      <c r="L10" s="39" t="inlineStr">
         <is>
           <t>Written  10</t>
         </is>
       </c>
-      <c r="M10" s="35" t="inlineStr">
+      <c r="M10" s="39" t="inlineStr">
         <is>
           <t>Practical 80</t>
         </is>
       </c>
-      <c r="N10" s="35" t="inlineStr">
+      <c r="N10" s="39" t="inlineStr">
         <is>
           <t>Total  90</t>
         </is>
       </c>
-      <c r="O10" s="35" t="inlineStr">
+      <c r="O10" s="39" t="inlineStr">
         <is>
           <t>Written   35</t>
         </is>
       </c>
-      <c r="P10" s="35" t="inlineStr">
+      <c r="P10" s="39" t="inlineStr">
         <is>
           <t>Practical 25</t>
         </is>
       </c>
-      <c r="Q10" s="35" t="inlineStr">
+      <c r="Q10" s="39" t="inlineStr">
         <is>
           <t>Total  60</t>
         </is>
       </c>
-      <c r="R10" s="35" t="inlineStr">
+      <c r="R10" s="39" t="inlineStr">
         <is>
           <t>Written      200</t>
         </is>
       </c>
-      <c r="S10" s="35" t="inlineStr">
+      <c r="S10" s="39" t="inlineStr">
         <is>
           <t>Written   105</t>
         </is>
       </c>
-      <c r="T10" s="35" t="inlineStr">
+      <c r="T10" s="39" t="inlineStr">
         <is>
           <t>Practical   45</t>
         </is>
       </c>
-      <c r="U10" s="35" t="inlineStr">
+      <c r="U10" s="39" t="inlineStr">
         <is>
           <t>Total          150</t>
         </is>
@@ -2976,30 +2976,30 @@
       <c r="W10" s="14" t="n"/>
       <c r="X10" s="15" t="n"/>
       <c r="Y10" s="15" t="n"/>
-      <c r="Z10" s="49" t="n"/>
+      <c r="Z10" s="38" t="n"/>
     </row>
     <row r="11" ht="21.6" customHeight="1" s="28">
-      <c r="A11" s="30" t="inlineStr">
+      <c r="A11" s="45" t="inlineStr">
         <is>
           <t>(a)</t>
         </is>
       </c>
-      <c r="B11" s="48" t="inlineStr">
+      <c r="B11" s="35" t="inlineStr">
         <is>
           <t>(b)</t>
         </is>
       </c>
-      <c r="C11" s="30" t="inlineStr">
+      <c r="C11" s="45" t="inlineStr">
         <is>
           <t>(c)</t>
         </is>
       </c>
-      <c r="D11" s="30" t="inlineStr">
+      <c r="D11" s="45" t="inlineStr">
         <is>
           <t>(d)</t>
         </is>
       </c>
-      <c r="E11" s="30" t="inlineStr">
+      <c r="E11" s="45" t="inlineStr">
         <is>
           <t>(e)</t>
         </is>
@@ -3009,7 +3009,7 @@
           <t>(f)</t>
         </is>
       </c>
-      <c r="G11" s="48" t="inlineStr">
+      <c r="G11" s="35" t="inlineStr">
         <is>
           <t>(g)</t>
         </is>
@@ -3019,17 +3019,17 @@
           <t>(h)</t>
         </is>
       </c>
-      <c r="I11" s="48" t="inlineStr">
+      <c r="I11" s="35" t="inlineStr">
         <is>
           <t>(j)</t>
         </is>
       </c>
-      <c r="J11" s="48" t="inlineStr">
+      <c r="J11" s="35" t="inlineStr">
         <is>
           <t>(k)</t>
         </is>
       </c>
-      <c r="K11" s="48" t="inlineStr">
+      <c r="K11" s="35" t="inlineStr">
         <is>
           <t>(l)</t>
         </is>
@@ -3084,63 +3084,63 @@
           <t>(v)</t>
         </is>
       </c>
-      <c r="V11" s="48" t="inlineStr">
+      <c r="V11" s="35" t="inlineStr">
         <is>
           <t>(w)</t>
         </is>
       </c>
-      <c r="W11" s="48" t="inlineStr">
+      <c r="W11" s="35" t="inlineStr">
         <is>
           <t>(x)</t>
         </is>
       </c>
-      <c r="X11" s="48" t="inlineStr">
+      <c r="X11" s="35" t="inlineStr">
         <is>
           <t>(y)</t>
         </is>
       </c>
-      <c r="Y11" s="48" t="inlineStr">
+      <c r="Y11" s="35" t="inlineStr">
         <is>
           <t>(z)</t>
         </is>
       </c>
-      <c r="Z11" s="30" t="inlineStr">
+      <c r="Z11" s="45" t="inlineStr">
         <is>
           <t>(aa)</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="49" t="n"/>
-      <c r="B12" s="48" t="inlineStr">
+      <c r="A12" s="38" t="n"/>
+      <c r="B12" s="35" t="inlineStr">
         <is>
           <t xml:space="preserve">NAME OF INSTITUTION : BHARAT MATA  H S SCHOOL, BILASPUR </t>
         </is>
       </c>
-      <c r="C12" s="40" t="n"/>
-      <c r="D12" s="40" t="n"/>
-      <c r="E12" s="40" t="n"/>
-      <c r="F12" s="40" t="n"/>
-      <c r="G12" s="40" t="n"/>
-      <c r="H12" s="40" t="n"/>
-      <c r="I12" s="40" t="n"/>
-      <c r="J12" s="40" t="n"/>
-      <c r="K12" s="40" t="n"/>
-      <c r="L12" s="40" t="n"/>
-      <c r="M12" s="40" t="n"/>
-      <c r="N12" s="40" t="n"/>
-      <c r="O12" s="40" t="n"/>
-      <c r="P12" s="40" t="n"/>
-      <c r="Q12" s="40" t="n"/>
-      <c r="R12" s="40" t="n"/>
-      <c r="S12" s="40" t="n"/>
-      <c r="T12" s="40" t="n"/>
-      <c r="U12" s="40" t="n"/>
-      <c r="V12" s="40" t="n"/>
-      <c r="W12" s="40" t="n"/>
-      <c r="X12" s="40" t="n"/>
-      <c r="Y12" s="40" t="n"/>
-      <c r="Z12" s="42" t="n"/>
+      <c r="C12" s="36" t="n"/>
+      <c r="D12" s="36" t="n"/>
+      <c r="E12" s="36" t="n"/>
+      <c r="F12" s="36" t="n"/>
+      <c r="G12" s="36" t="n"/>
+      <c r="H12" s="36" t="n"/>
+      <c r="I12" s="36" t="n"/>
+      <c r="J12" s="36" t="n"/>
+      <c r="K12" s="36" t="n"/>
+      <c r="L12" s="36" t="n"/>
+      <c r="M12" s="36" t="n"/>
+      <c r="N12" s="36" t="n"/>
+      <c r="O12" s="36" t="n"/>
+      <c r="P12" s="36" t="n"/>
+      <c r="Q12" s="36" t="n"/>
+      <c r="R12" s="36" t="n"/>
+      <c r="S12" s="36" t="n"/>
+      <c r="T12" s="36" t="n"/>
+      <c r="U12" s="36" t="n"/>
+      <c r="V12" s="36" t="n"/>
+      <c r="W12" s="36" t="n"/>
+      <c r="X12" s="36" t="n"/>
+      <c r="Y12" s="36" t="n"/>
+      <c r="Z12" s="37" t="n"/>
     </row>
     <row r="13" ht="55.5" customHeight="1" s="28">
       <c r="A13" s="1" t="n">
@@ -3190,45 +3190,45 @@
         <v>54</v>
       </c>
       <c r="L13" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="M13" s="49" t="n">
-        <v>70</v>
-      </c>
-      <c r="N13" s="49" t="n">
-        <v>76</v>
-      </c>
-      <c r="O13" s="49" t="n">
-        <v>23</v>
-      </c>
-      <c r="P13" s="49" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q13" s="49" t="n">
-        <v>38</v>
-      </c>
-      <c r="R13" s="49" t="n">
-        <v>180</v>
-      </c>
-      <c r="S13" s="49" t="n">
-        <v>79</v>
-      </c>
-      <c r="T13" s="49" t="n">
-        <v>41</v>
-      </c>
-      <c r="U13" s="49" t="n">
-        <v>130</v>
-      </c>
-      <c r="V13" s="49" t="n">
+        <v>5</v>
+      </c>
+      <c r="M13" s="38" t="n">
+        <v>75</v>
+      </c>
+      <c r="N13" s="38" t="n">
+        <v>45</v>
+      </c>
+      <c r="O13" s="38" t="n">
+        <v>30</v>
+      </c>
+      <c r="P13" s="38" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q13" s="38" t="n">
+        <v>60</v>
+      </c>
+      <c r="R13" s="38" t="n">
+        <v>200</v>
+      </c>
+      <c r="S13" s="38" t="n">
+        <v>105</v>
+      </c>
+      <c r="T13" s="38" t="n">
+        <v>45</v>
+      </c>
+      <c r="U13" s="38" t="n">
+        <v>150</v>
+      </c>
+      <c r="V13" s="38" t="n">
         <v>480</v>
       </c>
-      <c r="W13" s="49" t="n"/>
-      <c r="X13" s="49" t="n">
-        <v>375</v>
-      </c>
-      <c r="Y13" s="49" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="W13" s="38" t="n"/>
+      <c r="X13" s="38" t="n">
+        <v>480</v>
+      </c>
+      <c r="Y13" s="38" t="inlineStr">
+        <is>
+          <t>A</t>
         </is>
       </c>
       <c r="Z13" s="5" t="n"/>
@@ -3287,41 +3287,41 @@
       <c r="L14" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="M14" s="49" t="n">
+      <c r="M14" s="38" t="n">
         <v>85</v>
       </c>
-      <c r="N14" s="49" t="n">
+      <c r="N14" s="38" t="n">
         <v>68</v>
       </c>
-      <c r="O14" s="49" t="n">
+      <c r="O14" s="38" t="n">
         <v>6</v>
       </c>
-      <c r="P14" s="49" t="n">
+      <c r="P14" s="38" t="n">
         <v>6</v>
       </c>
-      <c r="Q14" s="49" t="n">
+      <c r="Q14" s="38" t="n">
         <v>57</v>
       </c>
-      <c r="R14" s="49" t="n">
+      <c r="R14" s="38" t="n">
         <v>190</v>
       </c>
-      <c r="S14" s="49" t="n">
+      <c r="S14" s="38" t="n">
         <v>6</v>
       </c>
-      <c r="T14" s="49" t="n">
+      <c r="T14" s="38" t="n">
         <v>35</v>
       </c>
-      <c r="U14" s="49" t="n">
+      <c r="U14" s="38" t="n">
         <v>150</v>
       </c>
-      <c r="V14" s="49" t="n">
+      <c r="V14" s="38" t="n">
         <v>200</v>
       </c>
-      <c r="W14" s="49" t="n"/>
-      <c r="X14" s="49" t="n">
+      <c r="W14" s="38" t="n"/>
+      <c r="X14" s="38" t="n">
         <v>200</v>
       </c>
-      <c r="Y14" s="49" t="inlineStr">
+      <c r="Y14" s="38" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
@@ -3382,43 +3382,43 @@
       <c r="L15" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="M15" s="49" t="n">
+      <c r="M15" s="38" t="n">
         <v>80</v>
       </c>
-      <c r="N15" s="49" t="n">
+      <c r="N15" s="38" t="n">
         <v>89</v>
       </c>
-      <c r="O15" s="49" t="n">
+      <c r="O15" s="38" t="n">
         <v>30</v>
       </c>
-      <c r="P15" s="49" t="n">
+      <c r="P15" s="38" t="n">
         <v>23</v>
       </c>
-      <c r="Q15" s="49" t="n">
+      <c r="Q15" s="38" t="n">
         <v>52</v>
       </c>
-      <c r="R15" s="49" t="n">
+      <c r="R15" s="38" t="n">
         <v>195</v>
       </c>
-      <c r="S15" s="49" t="n">
+      <c r="S15" s="38" t="n">
         <v>100</v>
       </c>
-      <c r="T15" s="49" t="n">
+      <c r="T15" s="38" t="n">
         <v>40</v>
       </c>
-      <c r="U15" s="49" t="n">
-        <v>157</v>
-      </c>
-      <c r="V15" s="49" t="n">
+      <c r="U15" s="38" t="n">
+        <v>150</v>
+      </c>
+      <c r="V15" s="38" t="n">
         <v>350</v>
       </c>
-      <c r="W15" s="49" t="n"/>
-      <c r="X15" s="49" t="n">
+      <c r="W15" s="38" t="n"/>
+      <c r="X15" s="38" t="n">
         <v>350</v>
       </c>
-      <c r="Y15" s="49" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="Y15" s="38" t="inlineStr">
+        <is>
+          <t>B</t>
         </is>
       </c>
       <c r="Z15" s="5" t="n"/>
@@ -3473,43 +3473,43 @@
       <c r="L16" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="M16" s="49" t="n">
+      <c r="M16" s="38" t="n">
         <v>51</v>
       </c>
-      <c r="N16" s="49" t="n">
+      <c r="N16" s="38" t="n">
         <v>82</v>
       </c>
-      <c r="O16" s="49" t="n">
+      <c r="O16" s="38" t="n">
         <v>30</v>
       </c>
-      <c r="P16" s="49" t="n">
+      <c r="P16" s="38" t="n">
         <v>23</v>
       </c>
-      <c r="Q16" s="49" t="n">
+      <c r="Q16" s="38" t="n">
         <v>54</v>
       </c>
-      <c r="R16" s="49" t="n">
-        <v>752</v>
-      </c>
-      <c r="S16" s="49" t="n">
+      <c r="R16" s="38" t="n">
+        <v>198</v>
+      </c>
+      <c r="S16" s="38" t="n">
         <v>100</v>
       </c>
-      <c r="T16" s="49" t="n">
+      <c r="T16" s="38" t="n">
         <v>40</v>
       </c>
-      <c r="U16" s="49" t="n">
-        <v>152</v>
-      </c>
-      <c r="V16" s="49" t="n">
+      <c r="U16" s="38" t="n">
+        <v>147</v>
+      </c>
+      <c r="V16" s="38" t="n">
         <v>323</v>
       </c>
-      <c r="W16" s="49" t="n"/>
-      <c r="X16" s="49" t="n">
-        <v>274</v>
-      </c>
-      <c r="Y16" s="49" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="W16" s="38" t="n"/>
+      <c r="X16" s="38" t="n">
+        <v>323</v>
+      </c>
+      <c r="Y16" s="38" t="inlineStr">
+        <is>
+          <t>B</t>
         </is>
       </c>
       <c r="Z16" s="5" t="n"/>
@@ -3562,29 +3562,29 @@
       <c r="J17" s="6" t="n"/>
       <c r="K17" s="6" t="n"/>
       <c r="L17" s="6" t="n"/>
-      <c r="M17" s="49" t="n"/>
-      <c r="N17" s="49" t="n">
+      <c r="M17" s="38" t="n"/>
+      <c r="N17" s="38" t="n">
         <v>78</v>
       </c>
-      <c r="O17" s="49" t="n"/>
-      <c r="P17" s="49" t="n"/>
-      <c r="Q17" s="49" t="n">
+      <c r="O17" s="38" t="n"/>
+      <c r="P17" s="38" t="n"/>
+      <c r="Q17" s="38" t="n">
         <v>35</v>
       </c>
-      <c r="R17" s="49" t="n">
+      <c r="R17" s="38" t="n">
         <v>735</v>
       </c>
-      <c r="S17" s="49" t="n"/>
-      <c r="T17" s="49" t="n"/>
-      <c r="U17" s="49" t="n">
+      <c r="S17" s="38" t="n"/>
+      <c r="T17" s="38" t="n"/>
+      <c r="U17" s="38" t="n">
         <v>123</v>
       </c>
-      <c r="V17" s="49" t="n">
+      <c r="V17" s="38" t="n">
         <v>380</v>
       </c>
-      <c r="W17" s="49" t="n"/>
-      <c r="X17" s="49" t="n"/>
-      <c r="Y17" s="49" t="inlineStr">
+      <c r="W17" s="38" t="n"/>
+      <c r="X17" s="38" t="n"/>
+      <c r="Y17" s="38" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -3639,19 +3639,19 @@
       <c r="J18" s="6" t="n"/>
       <c r="K18" s="6" t="n"/>
       <c r="L18" s="6" t="n"/>
-      <c r="M18" s="49" t="n"/>
-      <c r="N18" s="49" t="n"/>
-      <c r="O18" s="49" t="n"/>
-      <c r="P18" s="49" t="n"/>
-      <c r="Q18" s="49" t="n"/>
-      <c r="R18" s="49" t="n"/>
-      <c r="S18" s="49" t="n"/>
-      <c r="T18" s="49" t="n"/>
-      <c r="U18" s="49" t="n"/>
-      <c r="V18" s="49" t="n"/>
-      <c r="W18" s="49" t="n"/>
-      <c r="X18" s="49" t="n"/>
-      <c r="Y18" s="49" t="n"/>
+      <c r="M18" s="38" t="n"/>
+      <c r="N18" s="38" t="n"/>
+      <c r="O18" s="38" t="n"/>
+      <c r="P18" s="38" t="n"/>
+      <c r="Q18" s="38" t="n"/>
+      <c r="R18" s="38" t="n"/>
+      <c r="S18" s="38" t="n"/>
+      <c r="T18" s="38" t="n"/>
+      <c r="U18" s="38" t="n"/>
+      <c r="V18" s="38" t="n"/>
+      <c r="W18" s="38" t="n"/>
+      <c r="X18" s="38" t="n"/>
+      <c r="Y18" s="38" t="n"/>
       <c r="Z18" s="5" t="n"/>
     </row>
     <row r="19" ht="70.5" customHeight="1" s="28">
@@ -3702,19 +3702,19 @@
       <c r="J19" s="6" t="n"/>
       <c r="K19" s="6" t="n"/>
       <c r="L19" s="6" t="n"/>
-      <c r="M19" s="49" t="n"/>
-      <c r="N19" s="49" t="n"/>
-      <c r="O19" s="49" t="n"/>
-      <c r="P19" s="49" t="n"/>
-      <c r="Q19" s="49" t="n"/>
-      <c r="R19" s="49" t="n"/>
-      <c r="S19" s="49" t="n"/>
-      <c r="T19" s="49" t="n"/>
-      <c r="U19" s="49" t="n"/>
-      <c r="V19" s="49" t="n"/>
-      <c r="W19" s="49" t="n"/>
-      <c r="X19" s="49" t="n"/>
-      <c r="Y19" s="49" t="n"/>
+      <c r="M19" s="38" t="n"/>
+      <c r="N19" s="38" t="n"/>
+      <c r="O19" s="38" t="n"/>
+      <c r="P19" s="38" t="n"/>
+      <c r="Q19" s="38" t="n"/>
+      <c r="R19" s="38" t="n"/>
+      <c r="S19" s="38" t="n"/>
+      <c r="T19" s="38" t="n"/>
+      <c r="U19" s="38" t="n"/>
+      <c r="V19" s="38" t="n"/>
+      <c r="W19" s="38" t="n"/>
+      <c r="X19" s="38" t="n"/>
+      <c r="Y19" s="38" t="n"/>
       <c r="Z19" s="5" t="n"/>
     </row>
     <row r="20" ht="66" customHeight="1" s="28">
@@ -3765,19 +3765,19 @@
       <c r="J20" s="6" t="n"/>
       <c r="K20" s="6" t="n"/>
       <c r="L20" s="6" t="n"/>
-      <c r="M20" s="49" t="n"/>
-      <c r="N20" s="49" t="n"/>
-      <c r="O20" s="49" t="n"/>
-      <c r="P20" s="49" t="n"/>
-      <c r="Q20" s="49" t="n"/>
-      <c r="R20" s="49" t="n"/>
-      <c r="S20" s="49" t="n"/>
-      <c r="T20" s="49" t="n"/>
-      <c r="U20" s="49" t="n"/>
-      <c r="V20" s="49" t="n"/>
-      <c r="W20" s="49" t="n"/>
-      <c r="X20" s="49" t="n"/>
-      <c r="Y20" s="49" t="n"/>
+      <c r="M20" s="38" t="n"/>
+      <c r="N20" s="38" t="n"/>
+      <c r="O20" s="38" t="n"/>
+      <c r="P20" s="38" t="n"/>
+      <c r="Q20" s="38" t="n"/>
+      <c r="R20" s="38" t="n"/>
+      <c r="S20" s="38" t="n"/>
+      <c r="T20" s="38" t="n"/>
+      <c r="U20" s="38" t="n"/>
+      <c r="V20" s="38" t="n"/>
+      <c r="W20" s="38" t="n"/>
+      <c r="X20" s="38" t="n"/>
+      <c r="Y20" s="38" t="n"/>
       <c r="Z20" s="5" t="n"/>
     </row>
     <row r="21" ht="60" customHeight="1" s="28">
@@ -3828,19 +3828,19 @@
       <c r="J21" s="6" t="n"/>
       <c r="K21" s="6" t="n"/>
       <c r="L21" s="6" t="n"/>
-      <c r="M21" s="49" t="n"/>
-      <c r="N21" s="49" t="n"/>
-      <c r="O21" s="49" t="n"/>
-      <c r="P21" s="49" t="n"/>
-      <c r="Q21" s="49" t="n"/>
-      <c r="R21" s="49" t="n"/>
-      <c r="S21" s="49" t="n"/>
-      <c r="T21" s="49" t="n"/>
-      <c r="U21" s="49" t="n"/>
-      <c r="V21" s="49" t="n"/>
-      <c r="W21" s="49" t="n"/>
-      <c r="X21" s="49" t="n"/>
-      <c r="Y21" s="49" t="n"/>
+      <c r="M21" s="38" t="n"/>
+      <c r="N21" s="38" t="n"/>
+      <c r="O21" s="38" t="n"/>
+      <c r="P21" s="38" t="n"/>
+      <c r="Q21" s="38" t="n"/>
+      <c r="R21" s="38" t="n"/>
+      <c r="S21" s="38" t="n"/>
+      <c r="T21" s="38" t="n"/>
+      <c r="U21" s="38" t="n"/>
+      <c r="V21" s="38" t="n"/>
+      <c r="W21" s="38" t="n"/>
+      <c r="X21" s="38" t="n"/>
+      <c r="Y21" s="38" t="n"/>
       <c r="Z21" s="5" t="n"/>
     </row>
     <row r="22" ht="70.5" customHeight="1" s="28">
@@ -3891,19 +3891,19 @@
       <c r="J22" s="6" t="n"/>
       <c r="K22" s="6" t="n"/>
       <c r="L22" s="6" t="n"/>
-      <c r="M22" s="49" t="n"/>
-      <c r="N22" s="49" t="n"/>
-      <c r="O22" s="49" t="n"/>
-      <c r="P22" s="49" t="n"/>
-      <c r="Q22" s="49" t="n"/>
-      <c r="R22" s="49" t="n"/>
-      <c r="S22" s="49" t="n"/>
-      <c r="T22" s="49" t="n"/>
-      <c r="U22" s="49" t="n"/>
-      <c r="V22" s="49" t="n"/>
-      <c r="W22" s="49" t="n"/>
-      <c r="X22" s="49" t="n"/>
-      <c r="Y22" s="49" t="n"/>
+      <c r="M22" s="38" t="n"/>
+      <c r="N22" s="38" t="n"/>
+      <c r="O22" s="38" t="n"/>
+      <c r="P22" s="38" t="n"/>
+      <c r="Q22" s="38" t="n"/>
+      <c r="R22" s="38" t="n"/>
+      <c r="S22" s="38" t="n"/>
+      <c r="T22" s="38" t="n"/>
+      <c r="U22" s="38" t="n"/>
+      <c r="V22" s="38" t="n"/>
+      <c r="W22" s="38" t="n"/>
+      <c r="X22" s="38" t="n"/>
+      <c r="Y22" s="38" t="n"/>
       <c r="Z22" s="5" t="n"/>
     </row>
     <row r="23" ht="58.5" customHeight="1" s="28">
@@ -3954,19 +3954,19 @@
       <c r="J23" s="6" t="n"/>
       <c r="K23" s="6" t="n"/>
       <c r="L23" s="6" t="n"/>
-      <c r="M23" s="49" t="n"/>
-      <c r="N23" s="49" t="n"/>
-      <c r="O23" s="49" t="n"/>
-      <c r="P23" s="49" t="n"/>
-      <c r="Q23" s="49" t="n"/>
-      <c r="R23" s="49" t="n"/>
-      <c r="S23" s="49" t="n"/>
-      <c r="T23" s="49" t="n"/>
-      <c r="U23" s="49" t="n"/>
-      <c r="V23" s="49" t="n"/>
-      <c r="W23" s="49" t="n"/>
-      <c r="X23" s="49" t="n"/>
-      <c r="Y23" s="49" t="n"/>
+      <c r="M23" s="38" t="n"/>
+      <c r="N23" s="38" t="n"/>
+      <c r="O23" s="38" t="n"/>
+      <c r="P23" s="38" t="n"/>
+      <c r="Q23" s="38" t="n"/>
+      <c r="R23" s="38" t="n"/>
+      <c r="S23" s="38" t="n"/>
+      <c r="T23" s="38" t="n"/>
+      <c r="U23" s="38" t="n"/>
+      <c r="V23" s="38" t="n"/>
+      <c r="W23" s="38" t="n"/>
+      <c r="X23" s="38" t="n"/>
+      <c r="Y23" s="38" t="n"/>
       <c r="Z23" s="5" t="n"/>
     </row>
     <row r="24" ht="70.5" customHeight="1" s="28">
@@ -4017,19 +4017,19 @@
       <c r="J24" s="6" t="n"/>
       <c r="K24" s="6" t="n"/>
       <c r="L24" s="6" t="n"/>
-      <c r="M24" s="49" t="n"/>
-      <c r="N24" s="49" t="n"/>
-      <c r="O24" s="49" t="n"/>
-      <c r="P24" s="49" t="n"/>
-      <c r="Q24" s="49" t="n"/>
-      <c r="R24" s="49" t="n"/>
-      <c r="S24" s="49" t="n"/>
-      <c r="T24" s="49" t="n"/>
-      <c r="U24" s="49" t="n"/>
-      <c r="V24" s="49" t="n"/>
-      <c r="W24" s="49" t="n"/>
-      <c r="X24" s="49" t="n"/>
-      <c r="Y24" s="49" t="n"/>
+      <c r="M24" s="38" t="n"/>
+      <c r="N24" s="38" t="n"/>
+      <c r="O24" s="38" t="n"/>
+      <c r="P24" s="38" t="n"/>
+      <c r="Q24" s="38" t="n"/>
+      <c r="R24" s="38" t="n"/>
+      <c r="S24" s="38" t="n"/>
+      <c r="T24" s="38" t="n"/>
+      <c r="U24" s="38" t="n"/>
+      <c r="V24" s="38" t="n"/>
+      <c r="W24" s="38" t="n"/>
+      <c r="X24" s="38" t="n"/>
+      <c r="Y24" s="38" t="n"/>
       <c r="Z24" s="5" t="n"/>
     </row>
     <row r="25" ht="64.5" customHeight="1" s="28">
@@ -4080,19 +4080,19 @@
       <c r="J25" s="6" t="n"/>
       <c r="K25" s="6" t="n"/>
       <c r="L25" s="6" t="n"/>
-      <c r="M25" s="49" t="n"/>
-      <c r="N25" s="49" t="n"/>
-      <c r="O25" s="49" t="n"/>
-      <c r="P25" s="49" t="n"/>
-      <c r="Q25" s="49" t="n"/>
-      <c r="R25" s="49" t="n"/>
-      <c r="S25" s="49" t="n"/>
-      <c r="T25" s="49" t="n"/>
-      <c r="U25" s="49" t="n"/>
-      <c r="V25" s="49" t="n"/>
-      <c r="W25" s="49" t="n"/>
-      <c r="X25" s="49" t="n"/>
-      <c r="Y25" s="49" t="n"/>
+      <c r="M25" s="38" t="n"/>
+      <c r="N25" s="38" t="n"/>
+      <c r="O25" s="38" t="n"/>
+      <c r="P25" s="38" t="n"/>
+      <c r="Q25" s="38" t="n"/>
+      <c r="R25" s="38" t="n"/>
+      <c r="S25" s="38" t="n"/>
+      <c r="T25" s="38" t="n"/>
+      <c r="U25" s="38" t="n"/>
+      <c r="V25" s="38" t="n"/>
+      <c r="W25" s="38" t="n"/>
+      <c r="X25" s="38" t="n"/>
+      <c r="Y25" s="38" t="n"/>
       <c r="Z25" s="5" t="n"/>
     </row>
     <row r="26" ht="70.5" customHeight="1" s="28">
@@ -4143,19 +4143,19 @@
       <c r="J26" s="6" t="n"/>
       <c r="K26" s="6" t="n"/>
       <c r="L26" s="6" t="n"/>
-      <c r="M26" s="49" t="n"/>
-      <c r="N26" s="49" t="n"/>
-      <c r="O26" s="49" t="n"/>
-      <c r="P26" s="49" t="n"/>
-      <c r="Q26" s="49" t="n"/>
-      <c r="R26" s="49" t="n"/>
-      <c r="S26" s="49" t="n"/>
-      <c r="T26" s="49" t="n"/>
-      <c r="U26" s="49" t="n"/>
-      <c r="V26" s="49" t="n"/>
-      <c r="W26" s="49" t="n"/>
-      <c r="X26" s="49" t="n"/>
-      <c r="Y26" s="49" t="n"/>
+      <c r="M26" s="38" t="n"/>
+      <c r="N26" s="38" t="n"/>
+      <c r="O26" s="38" t="n"/>
+      <c r="P26" s="38" t="n"/>
+      <c r="Q26" s="38" t="n"/>
+      <c r="R26" s="38" t="n"/>
+      <c r="S26" s="38" t="n"/>
+      <c r="T26" s="38" t="n"/>
+      <c r="U26" s="38" t="n"/>
+      <c r="V26" s="38" t="n"/>
+      <c r="W26" s="38" t="n"/>
+      <c r="X26" s="38" t="n"/>
+      <c r="Y26" s="38" t="n"/>
       <c r="Z26" s="5" t="n"/>
     </row>
     <row r="27" ht="63" customHeight="1" s="28">
@@ -4206,19 +4206,19 @@
       <c r="J27" s="6" t="n"/>
       <c r="K27" s="6" t="n"/>
       <c r="L27" s="6" t="n"/>
-      <c r="M27" s="49" t="n"/>
-      <c r="N27" s="49" t="n"/>
-      <c r="O27" s="49" t="n"/>
-      <c r="P27" s="49" t="n"/>
-      <c r="Q27" s="49" t="n"/>
-      <c r="R27" s="49" t="n"/>
-      <c r="S27" s="49" t="n"/>
-      <c r="T27" s="49" t="n"/>
-      <c r="U27" s="49" t="n"/>
-      <c r="V27" s="49" t="n"/>
-      <c r="W27" s="49" t="n"/>
-      <c r="X27" s="49" t="n"/>
-      <c r="Y27" s="49" t="n"/>
+      <c r="M27" s="38" t="n"/>
+      <c r="N27" s="38" t="n"/>
+      <c r="O27" s="38" t="n"/>
+      <c r="P27" s="38" t="n"/>
+      <c r="Q27" s="38" t="n"/>
+      <c r="R27" s="38" t="n"/>
+      <c r="S27" s="38" t="n"/>
+      <c r="T27" s="38" t="n"/>
+      <c r="U27" s="38" t="n"/>
+      <c r="V27" s="38" t="n"/>
+      <c r="W27" s="38" t="n"/>
+      <c r="X27" s="38" t="n"/>
+      <c r="Y27" s="38" t="n"/>
       <c r="Z27" s="5" t="n"/>
     </row>
     <row r="28" ht="70.5" customHeight="1" s="28">
@@ -4269,19 +4269,19 @@
       <c r="J28" s="6" t="n"/>
       <c r="K28" s="6" t="n"/>
       <c r="L28" s="6" t="n"/>
-      <c r="M28" s="49" t="n"/>
-      <c r="N28" s="49" t="n"/>
-      <c r="O28" s="49" t="n"/>
-      <c r="P28" s="49" t="n"/>
-      <c r="Q28" s="49" t="n"/>
-      <c r="R28" s="49" t="n"/>
-      <c r="S28" s="49" t="n"/>
-      <c r="T28" s="49" t="n"/>
-      <c r="U28" s="49" t="n"/>
-      <c r="V28" s="49" t="n"/>
-      <c r="W28" s="49" t="n"/>
-      <c r="X28" s="49" t="n"/>
-      <c r="Y28" s="49" t="n"/>
+      <c r="M28" s="38" t="n"/>
+      <c r="N28" s="38" t="n"/>
+      <c r="O28" s="38" t="n"/>
+      <c r="P28" s="38" t="n"/>
+      <c r="Q28" s="38" t="n"/>
+      <c r="R28" s="38" t="n"/>
+      <c r="S28" s="38" t="n"/>
+      <c r="T28" s="38" t="n"/>
+      <c r="U28" s="38" t="n"/>
+      <c r="V28" s="38" t="n"/>
+      <c r="W28" s="38" t="n"/>
+      <c r="X28" s="38" t="n"/>
+      <c r="Y28" s="38" t="n"/>
       <c r="Z28" s="5" t="n"/>
     </row>
     <row r="29" ht="70.5" customHeight="1" s="28">
@@ -4332,19 +4332,19 @@
       <c r="J29" s="6" t="n"/>
       <c r="K29" s="6" t="n"/>
       <c r="L29" s="6" t="n"/>
-      <c r="M29" s="49" t="n"/>
-      <c r="N29" s="49" t="n"/>
-      <c r="O29" s="49" t="n"/>
-      <c r="P29" s="49" t="n"/>
-      <c r="Q29" s="49" t="n"/>
-      <c r="R29" s="49" t="n"/>
-      <c r="S29" s="49" t="n"/>
-      <c r="T29" s="49" t="n"/>
-      <c r="U29" s="49" t="n"/>
-      <c r="V29" s="49" t="n"/>
-      <c r="W29" s="49" t="n"/>
-      <c r="X29" s="49" t="n"/>
-      <c r="Y29" s="49" t="n"/>
+      <c r="M29" s="38" t="n"/>
+      <c r="N29" s="38" t="n"/>
+      <c r="O29" s="38" t="n"/>
+      <c r="P29" s="38" t="n"/>
+      <c r="Q29" s="38" t="n"/>
+      <c r="R29" s="38" t="n"/>
+      <c r="S29" s="38" t="n"/>
+      <c r="T29" s="38" t="n"/>
+      <c r="U29" s="38" t="n"/>
+      <c r="V29" s="38" t="n"/>
+      <c r="W29" s="38" t="n"/>
+      <c r="X29" s="38" t="n"/>
+      <c r="Y29" s="38" t="n"/>
       <c r="Z29" s="5" t="n"/>
     </row>
     <row r="30" ht="70.5" customHeight="1" s="28">
@@ -4395,19 +4395,19 @@
       <c r="J30" s="6" t="n"/>
       <c r="K30" s="6" t="n"/>
       <c r="L30" s="6" t="n"/>
-      <c r="M30" s="49" t="n"/>
-      <c r="N30" s="49" t="n"/>
-      <c r="O30" s="49" t="n"/>
-      <c r="P30" s="49" t="n"/>
-      <c r="Q30" s="49" t="n"/>
-      <c r="R30" s="49" t="n"/>
-      <c r="S30" s="49" t="n"/>
-      <c r="T30" s="49" t="n"/>
-      <c r="U30" s="49" t="n"/>
-      <c r="V30" s="49" t="n"/>
-      <c r="W30" s="49" t="n"/>
-      <c r="X30" s="49" t="n"/>
-      <c r="Y30" s="49" t="n"/>
+      <c r="M30" s="38" t="n"/>
+      <c r="N30" s="38" t="n"/>
+      <c r="O30" s="38" t="n"/>
+      <c r="P30" s="38" t="n"/>
+      <c r="Q30" s="38" t="n"/>
+      <c r="R30" s="38" t="n"/>
+      <c r="S30" s="38" t="n"/>
+      <c r="T30" s="38" t="n"/>
+      <c r="U30" s="38" t="n"/>
+      <c r="V30" s="38" t="n"/>
+      <c r="W30" s="38" t="n"/>
+      <c r="X30" s="38" t="n"/>
+      <c r="Y30" s="38" t="n"/>
       <c r="Z30" s="5" t="n"/>
     </row>
     <row r="31" ht="70.5" customHeight="1" s="28">
@@ -4458,19 +4458,19 @@
       <c r="J31" s="6" t="n"/>
       <c r="K31" s="6" t="n"/>
       <c r="L31" s="6" t="n"/>
-      <c r="M31" s="49" t="n"/>
-      <c r="N31" s="49" t="n"/>
-      <c r="O31" s="49" t="n"/>
-      <c r="P31" s="49" t="n"/>
-      <c r="Q31" s="49" t="n"/>
-      <c r="R31" s="49" t="n"/>
-      <c r="S31" s="49" t="n"/>
-      <c r="T31" s="49" t="n"/>
-      <c r="U31" s="49" t="n"/>
-      <c r="V31" s="49" t="n"/>
-      <c r="W31" s="49" t="n"/>
-      <c r="X31" s="49" t="n"/>
-      <c r="Y31" s="49" t="n"/>
+      <c r="M31" s="38" t="n"/>
+      <c r="N31" s="38" t="n"/>
+      <c r="O31" s="38" t="n"/>
+      <c r="P31" s="38" t="n"/>
+      <c r="Q31" s="38" t="n"/>
+      <c r="R31" s="38" t="n"/>
+      <c r="S31" s="38" t="n"/>
+      <c r="T31" s="38" t="n"/>
+      <c r="U31" s="38" t="n"/>
+      <c r="V31" s="38" t="n"/>
+      <c r="W31" s="38" t="n"/>
+      <c r="X31" s="38" t="n"/>
+      <c r="Y31" s="38" t="n"/>
       <c r="Z31" s="5" t="n"/>
     </row>
     <row r="32" ht="70.5" customHeight="1" s="28">
@@ -4521,19 +4521,19 @@
       <c r="J32" s="6" t="n"/>
       <c r="K32" s="6" t="n"/>
       <c r="L32" s="6" t="n"/>
-      <c r="M32" s="49" t="n"/>
-      <c r="N32" s="49" t="n"/>
-      <c r="O32" s="49" t="n"/>
-      <c r="P32" s="49" t="n"/>
-      <c r="Q32" s="49" t="n"/>
-      <c r="R32" s="49" t="n"/>
-      <c r="S32" s="49" t="n"/>
-      <c r="T32" s="49" t="n"/>
-      <c r="U32" s="49" t="n"/>
-      <c r="V32" s="49" t="n"/>
-      <c r="W32" s="49" t="n"/>
-      <c r="X32" s="49" t="n"/>
-      <c r="Y32" s="49" t="n"/>
+      <c r="M32" s="38" t="n"/>
+      <c r="N32" s="38" t="n"/>
+      <c r="O32" s="38" t="n"/>
+      <c r="P32" s="38" t="n"/>
+      <c r="Q32" s="38" t="n"/>
+      <c r="R32" s="38" t="n"/>
+      <c r="S32" s="38" t="n"/>
+      <c r="T32" s="38" t="n"/>
+      <c r="U32" s="38" t="n"/>
+      <c r="V32" s="38" t="n"/>
+      <c r="W32" s="38" t="n"/>
+      <c r="X32" s="38" t="n"/>
+      <c r="Y32" s="38" t="n"/>
       <c r="Z32" s="5" t="n"/>
     </row>
     <row r="33" ht="70.5" customHeight="1" s="28">
@@ -4584,19 +4584,19 @@
       <c r="J33" s="6" t="n"/>
       <c r="K33" s="6" t="n"/>
       <c r="L33" s="6" t="n"/>
-      <c r="M33" s="49" t="n"/>
-      <c r="N33" s="49" t="n"/>
-      <c r="O33" s="49" t="n"/>
-      <c r="P33" s="49" t="n"/>
-      <c r="Q33" s="49" t="n"/>
-      <c r="R33" s="49" t="n"/>
-      <c r="S33" s="49" t="n"/>
-      <c r="T33" s="49" t="n"/>
-      <c r="U33" s="49" t="n"/>
-      <c r="V33" s="49" t="n"/>
-      <c r="W33" s="49" t="n"/>
-      <c r="X33" s="49" t="n"/>
-      <c r="Y33" s="49" t="n"/>
+      <c r="M33" s="38" t="n"/>
+      <c r="N33" s="38" t="n"/>
+      <c r="O33" s="38" t="n"/>
+      <c r="P33" s="38" t="n"/>
+      <c r="Q33" s="38" t="n"/>
+      <c r="R33" s="38" t="n"/>
+      <c r="S33" s="38" t="n"/>
+      <c r="T33" s="38" t="n"/>
+      <c r="U33" s="38" t="n"/>
+      <c r="V33" s="38" t="n"/>
+      <c r="W33" s="38" t="n"/>
+      <c r="X33" s="38" t="n"/>
+      <c r="Y33" s="38" t="n"/>
       <c r="Z33" s="5" t="n"/>
     </row>
     <row r="34" ht="75.75" customHeight="1" s="28">
@@ -4647,19 +4647,19 @@
       <c r="J34" s="6" t="n"/>
       <c r="K34" s="6" t="n"/>
       <c r="L34" s="6" t="n"/>
-      <c r="M34" s="49" t="n"/>
-      <c r="N34" s="49" t="n"/>
-      <c r="O34" s="49" t="n"/>
-      <c r="P34" s="49" t="n"/>
-      <c r="Q34" s="49" t="n"/>
-      <c r="R34" s="49" t="n"/>
-      <c r="S34" s="49" t="n"/>
-      <c r="T34" s="49" t="n"/>
-      <c r="U34" s="49" t="n"/>
-      <c r="V34" s="49" t="n"/>
-      <c r="W34" s="49" t="n"/>
-      <c r="X34" s="49" t="n"/>
-      <c r="Y34" s="49" t="n"/>
+      <c r="M34" s="38" t="n"/>
+      <c r="N34" s="38" t="n"/>
+      <c r="O34" s="38" t="n"/>
+      <c r="P34" s="38" t="n"/>
+      <c r="Q34" s="38" t="n"/>
+      <c r="R34" s="38" t="n"/>
+      <c r="S34" s="38" t="n"/>
+      <c r="T34" s="38" t="n"/>
+      <c r="U34" s="38" t="n"/>
+      <c r="V34" s="38" t="n"/>
+      <c r="W34" s="38" t="n"/>
+      <c r="X34" s="38" t="n"/>
+      <c r="Y34" s="38" t="n"/>
       <c r="Z34" s="5" t="n"/>
     </row>
     <row r="35" ht="60.75" customHeight="1" s="28">
@@ -4710,19 +4710,19 @@
       <c r="J35" s="6" t="n"/>
       <c r="K35" s="6" t="n"/>
       <c r="L35" s="6" t="n"/>
-      <c r="M35" s="49" t="n"/>
-      <c r="N35" s="49" t="n"/>
-      <c r="O35" s="49" t="n"/>
-      <c r="P35" s="49" t="n"/>
-      <c r="Q35" s="49" t="n"/>
-      <c r="R35" s="49" t="n"/>
-      <c r="S35" s="49" t="n"/>
-      <c r="T35" s="49" t="n"/>
-      <c r="U35" s="49" t="n"/>
-      <c r="V35" s="49" t="n"/>
-      <c r="W35" s="49" t="n"/>
-      <c r="X35" s="49" t="n"/>
-      <c r="Y35" s="49" t="n"/>
+      <c r="M35" s="38" t="n"/>
+      <c r="N35" s="38" t="n"/>
+      <c r="O35" s="38" t="n"/>
+      <c r="P35" s="38" t="n"/>
+      <c r="Q35" s="38" t="n"/>
+      <c r="R35" s="38" t="n"/>
+      <c r="S35" s="38" t="n"/>
+      <c r="T35" s="38" t="n"/>
+      <c r="U35" s="38" t="n"/>
+      <c r="V35" s="38" t="n"/>
+      <c r="W35" s="38" t="n"/>
+      <c r="X35" s="38" t="n"/>
+      <c r="Y35" s="38" t="n"/>
       <c r="Z35" s="5" t="n"/>
     </row>
     <row r="36" ht="60" customHeight="1" s="28">
@@ -4773,19 +4773,19 @@
       <c r="J36" s="6" t="n"/>
       <c r="K36" s="6" t="n"/>
       <c r="L36" s="6" t="n"/>
-      <c r="M36" s="49" t="n"/>
-      <c r="N36" s="49" t="n"/>
-      <c r="O36" s="49" t="n"/>
-      <c r="P36" s="49" t="n"/>
-      <c r="Q36" s="49" t="n"/>
-      <c r="R36" s="49" t="n"/>
-      <c r="S36" s="49" t="n"/>
-      <c r="T36" s="49" t="n"/>
-      <c r="U36" s="49" t="n"/>
-      <c r="V36" s="49" t="n"/>
-      <c r="W36" s="49" t="n"/>
-      <c r="X36" s="49" t="n"/>
-      <c r="Y36" s="49" t="n"/>
+      <c r="M36" s="38" t="n"/>
+      <c r="N36" s="38" t="n"/>
+      <c r="O36" s="38" t="n"/>
+      <c r="P36" s="38" t="n"/>
+      <c r="Q36" s="38" t="n"/>
+      <c r="R36" s="38" t="n"/>
+      <c r="S36" s="38" t="n"/>
+      <c r="T36" s="38" t="n"/>
+      <c r="U36" s="38" t="n"/>
+      <c r="V36" s="38" t="n"/>
+      <c r="W36" s="38" t="n"/>
+      <c r="X36" s="38" t="n"/>
+      <c r="Y36" s="38" t="n"/>
       <c r="Z36" s="5" t="n"/>
     </row>
     <row r="37" ht="70.5" customHeight="1" s="28">
@@ -4836,19 +4836,19 @@
       <c r="J37" s="6" t="n"/>
       <c r="K37" s="6" t="n"/>
       <c r="L37" s="6" t="n"/>
-      <c r="M37" s="49" t="n"/>
-      <c r="N37" s="49" t="n"/>
-      <c r="O37" s="49" t="n"/>
-      <c r="P37" s="49" t="n"/>
-      <c r="Q37" s="49" t="n"/>
-      <c r="R37" s="49" t="n"/>
-      <c r="S37" s="49" t="n"/>
-      <c r="T37" s="49" t="n"/>
-      <c r="U37" s="49" t="n"/>
-      <c r="V37" s="49" t="n"/>
-      <c r="W37" s="49" t="n"/>
-      <c r="X37" s="49" t="n"/>
-      <c r="Y37" s="49" t="n"/>
+      <c r="M37" s="38" t="n"/>
+      <c r="N37" s="38" t="n"/>
+      <c r="O37" s="38" t="n"/>
+      <c r="P37" s="38" t="n"/>
+      <c r="Q37" s="38" t="n"/>
+      <c r="R37" s="38" t="n"/>
+      <c r="S37" s="38" t="n"/>
+      <c r="T37" s="38" t="n"/>
+      <c r="U37" s="38" t="n"/>
+      <c r="V37" s="38" t="n"/>
+      <c r="W37" s="38" t="n"/>
+      <c r="X37" s="38" t="n"/>
+      <c r="Y37" s="38" t="n"/>
       <c r="Z37" s="5" t="n"/>
     </row>
     <row r="38" ht="70.5" customHeight="1" s="28">
@@ -4899,19 +4899,19 @@
       <c r="J38" s="6" t="n"/>
       <c r="K38" s="6" t="n"/>
       <c r="L38" s="6" t="n"/>
-      <c r="M38" s="49" t="n"/>
-      <c r="N38" s="49" t="n"/>
-      <c r="O38" s="49" t="n"/>
-      <c r="P38" s="49" t="n"/>
-      <c r="Q38" s="49" t="n"/>
-      <c r="R38" s="49" t="n"/>
-      <c r="S38" s="49" t="n"/>
-      <c r="T38" s="49" t="n"/>
-      <c r="U38" s="49" t="n"/>
-      <c r="V38" s="49" t="n"/>
-      <c r="W38" s="49" t="n"/>
-      <c r="X38" s="49" t="n"/>
-      <c r="Y38" s="49" t="n"/>
+      <c r="M38" s="38" t="n"/>
+      <c r="N38" s="38" t="n"/>
+      <c r="O38" s="38" t="n"/>
+      <c r="P38" s="38" t="n"/>
+      <c r="Q38" s="38" t="n"/>
+      <c r="R38" s="38" t="n"/>
+      <c r="S38" s="38" t="n"/>
+      <c r="T38" s="38" t="n"/>
+      <c r="U38" s="38" t="n"/>
+      <c r="V38" s="38" t="n"/>
+      <c r="W38" s="38" t="n"/>
+      <c r="X38" s="38" t="n"/>
+      <c r="Y38" s="38" t="n"/>
       <c r="Z38" s="5" t="n"/>
     </row>
     <row r="39" ht="58.5" customHeight="1" s="28">
@@ -4962,19 +4962,19 @@
       <c r="J39" s="6" t="n"/>
       <c r="K39" s="6" t="n"/>
       <c r="L39" s="6" t="n"/>
-      <c r="M39" s="49" t="n"/>
-      <c r="N39" s="49" t="n"/>
-      <c r="O39" s="49" t="n"/>
-      <c r="P39" s="49" t="n"/>
-      <c r="Q39" s="49" t="n"/>
-      <c r="R39" s="49" t="n"/>
-      <c r="S39" s="49" t="n"/>
-      <c r="T39" s="49" t="n"/>
-      <c r="U39" s="49" t="n"/>
-      <c r="V39" s="49" t="n"/>
-      <c r="W39" s="49" t="n"/>
-      <c r="X39" s="49" t="n"/>
-      <c r="Y39" s="49" t="n"/>
+      <c r="M39" s="38" t="n"/>
+      <c r="N39" s="38" t="n"/>
+      <c r="O39" s="38" t="n"/>
+      <c r="P39" s="38" t="n"/>
+      <c r="Q39" s="38" t="n"/>
+      <c r="R39" s="38" t="n"/>
+      <c r="S39" s="38" t="n"/>
+      <c r="T39" s="38" t="n"/>
+      <c r="U39" s="38" t="n"/>
+      <c r="V39" s="38" t="n"/>
+      <c r="W39" s="38" t="n"/>
+      <c r="X39" s="38" t="n"/>
+      <c r="Y39" s="38" t="n"/>
       <c r="Z39" s="5" t="n"/>
     </row>
     <row r="40" ht="70.5" customHeight="1" s="28">
@@ -5025,19 +5025,19 @@
       <c r="J40" s="6" t="n"/>
       <c r="K40" s="6" t="n"/>
       <c r="L40" s="6" t="n"/>
-      <c r="M40" s="49" t="n"/>
-      <c r="N40" s="49" t="n"/>
-      <c r="O40" s="49" t="n"/>
-      <c r="P40" s="49" t="n"/>
-      <c r="Q40" s="49" t="n"/>
-      <c r="R40" s="49" t="n"/>
-      <c r="S40" s="49" t="n"/>
-      <c r="T40" s="49" t="n"/>
-      <c r="U40" s="49" t="n"/>
-      <c r="V40" s="49" t="n"/>
-      <c r="W40" s="49" t="n"/>
-      <c r="X40" s="49" t="n"/>
-      <c r="Y40" s="49" t="n"/>
+      <c r="M40" s="38" t="n"/>
+      <c r="N40" s="38" t="n"/>
+      <c r="O40" s="38" t="n"/>
+      <c r="P40" s="38" t="n"/>
+      <c r="Q40" s="38" t="n"/>
+      <c r="R40" s="38" t="n"/>
+      <c r="S40" s="38" t="n"/>
+      <c r="T40" s="38" t="n"/>
+      <c r="U40" s="38" t="n"/>
+      <c r="V40" s="38" t="n"/>
+      <c r="W40" s="38" t="n"/>
+      <c r="X40" s="38" t="n"/>
+      <c r="Y40" s="38" t="n"/>
       <c r="Z40" s="5" t="n"/>
     </row>
     <row r="41" ht="70.5" customHeight="1" s="28">
@@ -5088,19 +5088,19 @@
       <c r="J41" s="6" t="n"/>
       <c r="K41" s="6" t="n"/>
       <c r="L41" s="6" t="n"/>
-      <c r="M41" s="49" t="n"/>
-      <c r="N41" s="49" t="n"/>
-      <c r="O41" s="49" t="n"/>
-      <c r="P41" s="49" t="n"/>
-      <c r="Q41" s="49" t="n"/>
-      <c r="R41" s="49" t="n"/>
-      <c r="S41" s="49" t="n"/>
-      <c r="T41" s="49" t="n"/>
-      <c r="U41" s="49" t="n"/>
-      <c r="V41" s="49" t="n"/>
-      <c r="W41" s="49" t="n"/>
-      <c r="X41" s="49" t="n"/>
-      <c r="Y41" s="49" t="n"/>
+      <c r="M41" s="38" t="n"/>
+      <c r="N41" s="38" t="n"/>
+      <c r="O41" s="38" t="n"/>
+      <c r="P41" s="38" t="n"/>
+      <c r="Q41" s="38" t="n"/>
+      <c r="R41" s="38" t="n"/>
+      <c r="S41" s="38" t="n"/>
+      <c r="T41" s="38" t="n"/>
+      <c r="U41" s="38" t="n"/>
+      <c r="V41" s="38" t="n"/>
+      <c r="W41" s="38" t="n"/>
+      <c r="X41" s="38" t="n"/>
+      <c r="Y41" s="38" t="n"/>
       <c r="Z41" s="5" t="n"/>
     </row>
     <row r="42" ht="75.75" customHeight="1" s="28">
@@ -5151,19 +5151,19 @@
       <c r="J42" s="6" t="n"/>
       <c r="K42" s="6" t="n"/>
       <c r="L42" s="6" t="n"/>
-      <c r="M42" s="49" t="n"/>
-      <c r="N42" s="49" t="n"/>
-      <c r="O42" s="49" t="n"/>
-      <c r="P42" s="49" t="n"/>
-      <c r="Q42" s="49" t="n"/>
-      <c r="R42" s="49" t="n"/>
-      <c r="S42" s="49" t="n"/>
-      <c r="T42" s="49" t="n"/>
-      <c r="U42" s="49" t="n"/>
-      <c r="V42" s="49" t="n"/>
-      <c r="W42" s="49" t="n"/>
-      <c r="X42" s="49" t="n"/>
-      <c r="Y42" s="49" t="n"/>
+      <c r="M42" s="38" t="n"/>
+      <c r="N42" s="38" t="n"/>
+      <c r="O42" s="38" t="n"/>
+      <c r="P42" s="38" t="n"/>
+      <c r="Q42" s="38" t="n"/>
+      <c r="R42" s="38" t="n"/>
+      <c r="S42" s="38" t="n"/>
+      <c r="T42" s="38" t="n"/>
+      <c r="U42" s="38" t="n"/>
+      <c r="V42" s="38" t="n"/>
+      <c r="W42" s="38" t="n"/>
+      <c r="X42" s="38" t="n"/>
+      <c r="Y42" s="38" t="n"/>
       <c r="Z42" s="5" t="n"/>
     </row>
     <row r="43" ht="70.5" customHeight="1" s="28">
@@ -5214,19 +5214,19 @@
       <c r="J43" s="6" t="n"/>
       <c r="K43" s="6" t="n"/>
       <c r="L43" s="6" t="n"/>
-      <c r="M43" s="49" t="n"/>
-      <c r="N43" s="49" t="n"/>
-      <c r="O43" s="49" t="n"/>
-      <c r="P43" s="49" t="n"/>
-      <c r="Q43" s="49" t="n"/>
-      <c r="R43" s="49" t="n"/>
-      <c r="S43" s="49" t="n"/>
-      <c r="T43" s="49" t="n"/>
-      <c r="U43" s="49" t="n"/>
-      <c r="V43" s="49" t="n"/>
-      <c r="W43" s="49" t="n"/>
-      <c r="X43" s="49" t="n"/>
-      <c r="Y43" s="49" t="n"/>
+      <c r="M43" s="38" t="n"/>
+      <c r="N43" s="38" t="n"/>
+      <c r="O43" s="38" t="n"/>
+      <c r="P43" s="38" t="n"/>
+      <c r="Q43" s="38" t="n"/>
+      <c r="R43" s="38" t="n"/>
+      <c r="S43" s="38" t="n"/>
+      <c r="T43" s="38" t="n"/>
+      <c r="U43" s="38" t="n"/>
+      <c r="V43" s="38" t="n"/>
+      <c r="W43" s="38" t="n"/>
+      <c r="X43" s="38" t="n"/>
+      <c r="Y43" s="38" t="n"/>
       <c r="Z43" s="5" t="n"/>
     </row>
     <row r="44" ht="70.5" customHeight="1" s="28">
@@ -5277,19 +5277,19 @@
       <c r="J44" s="6" t="n"/>
       <c r="K44" s="6" t="n"/>
       <c r="L44" s="6" t="n"/>
-      <c r="M44" s="49" t="n"/>
-      <c r="N44" s="49" t="n"/>
-      <c r="O44" s="49" t="n"/>
-      <c r="P44" s="49" t="n"/>
-      <c r="Q44" s="49" t="n"/>
-      <c r="R44" s="49" t="n"/>
-      <c r="S44" s="49" t="n"/>
-      <c r="T44" s="49" t="n"/>
-      <c r="U44" s="49" t="n"/>
-      <c r="V44" s="49" t="n"/>
-      <c r="W44" s="49" t="n"/>
-      <c r="X44" s="49" t="n"/>
-      <c r="Y44" s="49" t="n"/>
+      <c r="M44" s="38" t="n"/>
+      <c r="N44" s="38" t="n"/>
+      <c r="O44" s="38" t="n"/>
+      <c r="P44" s="38" t="n"/>
+      <c r="Q44" s="38" t="n"/>
+      <c r="R44" s="38" t="n"/>
+      <c r="S44" s="38" t="n"/>
+      <c r="T44" s="38" t="n"/>
+      <c r="U44" s="38" t="n"/>
+      <c r="V44" s="38" t="n"/>
+      <c r="W44" s="38" t="n"/>
+      <c r="X44" s="38" t="n"/>
+      <c r="Y44" s="38" t="n"/>
       <c r="Z44" s="5" t="n"/>
     </row>
     <row r="45" ht="70.5" customHeight="1" s="28">
@@ -5340,19 +5340,19 @@
       <c r="J45" s="6" t="n"/>
       <c r="K45" s="6" t="n"/>
       <c r="L45" s="6" t="n"/>
-      <c r="M45" s="49" t="n"/>
-      <c r="N45" s="49" t="n"/>
-      <c r="O45" s="49" t="n"/>
-      <c r="P45" s="49" t="n"/>
-      <c r="Q45" s="49" t="n"/>
-      <c r="R45" s="49" t="n"/>
-      <c r="S45" s="49" t="n"/>
-      <c r="T45" s="49" t="n"/>
-      <c r="U45" s="49" t="n"/>
-      <c r="V45" s="49" t="n"/>
-      <c r="W45" s="49" t="n"/>
-      <c r="X45" s="49" t="n"/>
-      <c r="Y45" s="49" t="n"/>
+      <c r="M45" s="38" t="n"/>
+      <c r="N45" s="38" t="n"/>
+      <c r="O45" s="38" t="n"/>
+      <c r="P45" s="38" t="n"/>
+      <c r="Q45" s="38" t="n"/>
+      <c r="R45" s="38" t="n"/>
+      <c r="S45" s="38" t="n"/>
+      <c r="T45" s="38" t="n"/>
+      <c r="U45" s="38" t="n"/>
+      <c r="V45" s="38" t="n"/>
+      <c r="W45" s="38" t="n"/>
+      <c r="X45" s="38" t="n"/>
+      <c r="Y45" s="38" t="n"/>
       <c r="Z45" s="5" t="n"/>
     </row>
     <row r="46" ht="70.5" customHeight="1" s="28">
@@ -5403,19 +5403,19 @@
       <c r="J46" s="6" t="n"/>
       <c r="K46" s="6" t="n"/>
       <c r="L46" s="6" t="n"/>
-      <c r="M46" s="49" t="n"/>
-      <c r="N46" s="49" t="n"/>
-      <c r="O46" s="49" t="n"/>
-      <c r="P46" s="49" t="n"/>
-      <c r="Q46" s="49" t="n"/>
-      <c r="R46" s="49" t="n"/>
-      <c r="S46" s="49" t="n"/>
-      <c r="T46" s="49" t="n"/>
-      <c r="U46" s="49" t="n"/>
-      <c r="V46" s="49" t="n"/>
-      <c r="W46" s="49" t="n"/>
-      <c r="X46" s="49" t="n"/>
-      <c r="Y46" s="49" t="n"/>
+      <c r="M46" s="38" t="n"/>
+      <c r="N46" s="38" t="n"/>
+      <c r="O46" s="38" t="n"/>
+      <c r="P46" s="38" t="n"/>
+      <c r="Q46" s="38" t="n"/>
+      <c r="R46" s="38" t="n"/>
+      <c r="S46" s="38" t="n"/>
+      <c r="T46" s="38" t="n"/>
+      <c r="U46" s="38" t="n"/>
+      <c r="V46" s="38" t="n"/>
+      <c r="W46" s="38" t="n"/>
+      <c r="X46" s="38" t="n"/>
+      <c r="Y46" s="38" t="n"/>
       <c r="Z46" s="5" t="n"/>
     </row>
     <row r="47" ht="70.5" customHeight="1" s="28">
@@ -5466,19 +5466,19 @@
       <c r="J47" s="6" t="n"/>
       <c r="K47" s="6" t="n"/>
       <c r="L47" s="6" t="n"/>
-      <c r="M47" s="49" t="n"/>
-      <c r="N47" s="49" t="n"/>
-      <c r="O47" s="49" t="n"/>
-      <c r="P47" s="49" t="n"/>
-      <c r="Q47" s="49" t="n"/>
-      <c r="R47" s="49" t="n"/>
-      <c r="S47" s="49" t="n"/>
-      <c r="T47" s="49" t="n"/>
-      <c r="U47" s="49" t="n"/>
-      <c r="V47" s="49" t="n"/>
-      <c r="W47" s="49" t="n"/>
-      <c r="X47" s="49" t="n"/>
-      <c r="Y47" s="49" t="n"/>
+      <c r="M47" s="38" t="n"/>
+      <c r="N47" s="38" t="n"/>
+      <c r="O47" s="38" t="n"/>
+      <c r="P47" s="38" t="n"/>
+      <c r="Q47" s="38" t="n"/>
+      <c r="R47" s="38" t="n"/>
+      <c r="S47" s="38" t="n"/>
+      <c r="T47" s="38" t="n"/>
+      <c r="U47" s="38" t="n"/>
+      <c r="V47" s="38" t="n"/>
+      <c r="W47" s="38" t="n"/>
+      <c r="X47" s="38" t="n"/>
+      <c r="Y47" s="38" t="n"/>
       <c r="Z47" s="5" t="n"/>
     </row>
     <row r="48" ht="70.5" customHeight="1" s="28">
@@ -5529,19 +5529,19 @@
       <c r="J48" s="6" t="n"/>
       <c r="K48" s="6" t="n"/>
       <c r="L48" s="6" t="n"/>
-      <c r="M48" s="49" t="n"/>
-      <c r="N48" s="49" t="n"/>
-      <c r="O48" s="49" t="n"/>
-      <c r="P48" s="49" t="n"/>
-      <c r="Q48" s="49" t="n"/>
-      <c r="R48" s="49" t="n"/>
-      <c r="S48" s="49" t="n"/>
-      <c r="T48" s="49" t="n"/>
-      <c r="U48" s="49" t="n"/>
-      <c r="V48" s="49" t="n"/>
-      <c r="W48" s="49" t="n"/>
-      <c r="X48" s="49" t="n"/>
-      <c r="Y48" s="49" t="n"/>
+      <c r="M48" s="38" t="n"/>
+      <c r="N48" s="38" t="n"/>
+      <c r="O48" s="38" t="n"/>
+      <c r="P48" s="38" t="n"/>
+      <c r="Q48" s="38" t="n"/>
+      <c r="R48" s="38" t="n"/>
+      <c r="S48" s="38" t="n"/>
+      <c r="T48" s="38" t="n"/>
+      <c r="U48" s="38" t="n"/>
+      <c r="V48" s="38" t="n"/>
+      <c r="W48" s="38" t="n"/>
+      <c r="X48" s="38" t="n"/>
+      <c r="Y48" s="38" t="n"/>
       <c r="Z48" s="5" t="n"/>
     </row>
     <row r="49" ht="70.5" customHeight="1" s="28">
@@ -5592,19 +5592,19 @@
       <c r="J49" s="6" t="n"/>
       <c r="K49" s="6" t="n"/>
       <c r="L49" s="6" t="n"/>
-      <c r="M49" s="49" t="n"/>
-      <c r="N49" s="49" t="n"/>
-      <c r="O49" s="49" t="n"/>
-      <c r="P49" s="49" t="n"/>
-      <c r="Q49" s="49" t="n"/>
-      <c r="R49" s="49" t="n"/>
-      <c r="S49" s="49" t="n"/>
-      <c r="T49" s="49" t="n"/>
-      <c r="U49" s="49" t="n"/>
-      <c r="V49" s="49" t="n"/>
-      <c r="W49" s="49" t="n"/>
-      <c r="X49" s="49" t="n"/>
-      <c r="Y49" s="49" t="n"/>
+      <c r="M49" s="38" t="n"/>
+      <c r="N49" s="38" t="n"/>
+      <c r="O49" s="38" t="n"/>
+      <c r="P49" s="38" t="n"/>
+      <c r="Q49" s="38" t="n"/>
+      <c r="R49" s="38" t="n"/>
+      <c r="S49" s="38" t="n"/>
+      <c r="T49" s="38" t="n"/>
+      <c r="U49" s="38" t="n"/>
+      <c r="V49" s="38" t="n"/>
+      <c r="W49" s="38" t="n"/>
+      <c r="X49" s="38" t="n"/>
+      <c r="Y49" s="38" t="n"/>
       <c r="Z49" s="5" t="n"/>
     </row>
     <row r="50" ht="60" customHeight="1" s="28">
@@ -5655,19 +5655,19 @@
       <c r="J50" s="6" t="n"/>
       <c r="K50" s="6" t="n"/>
       <c r="L50" s="6" t="n"/>
-      <c r="M50" s="49" t="n"/>
-      <c r="N50" s="49" t="n"/>
-      <c r="O50" s="49" t="n"/>
-      <c r="P50" s="49" t="n"/>
-      <c r="Q50" s="49" t="n"/>
-      <c r="R50" s="49" t="n"/>
-      <c r="S50" s="49" t="n"/>
-      <c r="T50" s="49" t="n"/>
-      <c r="U50" s="49" t="n"/>
-      <c r="V50" s="49" t="n"/>
-      <c r="W50" s="49" t="n"/>
-      <c r="X50" s="49" t="n"/>
-      <c r="Y50" s="49" t="n"/>
+      <c r="M50" s="38" t="n"/>
+      <c r="N50" s="38" t="n"/>
+      <c r="O50" s="38" t="n"/>
+      <c r="P50" s="38" t="n"/>
+      <c r="Q50" s="38" t="n"/>
+      <c r="R50" s="38" t="n"/>
+      <c r="S50" s="38" t="n"/>
+      <c r="T50" s="38" t="n"/>
+      <c r="U50" s="38" t="n"/>
+      <c r="V50" s="38" t="n"/>
+      <c r="W50" s="38" t="n"/>
+      <c r="X50" s="38" t="n"/>
+      <c r="Y50" s="38" t="n"/>
       <c r="Z50" s="5" t="n"/>
     </row>
     <row r="51" ht="74.25" customHeight="1" s="28">
@@ -5718,19 +5718,19 @@
       <c r="J51" s="6" t="n"/>
       <c r="K51" s="6" t="n"/>
       <c r="L51" s="6" t="n"/>
-      <c r="M51" s="49" t="n"/>
-      <c r="N51" s="49" t="n"/>
-      <c r="O51" s="49" t="n"/>
-      <c r="P51" s="49" t="n"/>
-      <c r="Q51" s="49" t="n"/>
-      <c r="R51" s="49" t="n"/>
-      <c r="S51" s="49" t="n"/>
-      <c r="T51" s="49" t="n"/>
-      <c r="U51" s="49" t="n"/>
-      <c r="V51" s="49" t="n"/>
-      <c r="W51" s="49" t="n"/>
-      <c r="X51" s="49" t="n"/>
-      <c r="Y51" s="49" t="n"/>
+      <c r="M51" s="38" t="n"/>
+      <c r="N51" s="38" t="n"/>
+      <c r="O51" s="38" t="n"/>
+      <c r="P51" s="38" t="n"/>
+      <c r="Q51" s="38" t="n"/>
+      <c r="R51" s="38" t="n"/>
+      <c r="S51" s="38" t="n"/>
+      <c r="T51" s="38" t="n"/>
+      <c r="U51" s="38" t="n"/>
+      <c r="V51" s="38" t="n"/>
+      <c r="W51" s="38" t="n"/>
+      <c r="X51" s="38" t="n"/>
+      <c r="Y51" s="38" t="n"/>
       <c r="Z51" s="5" t="n"/>
     </row>
     <row r="52" ht="72" customHeight="1" s="28">
@@ -6238,14 +6238,14 @@
       <c r="Z59" s="10" t="n"/>
     </row>
     <row r="61">
-      <c r="B61" s="51" t="inlineStr">
+      <c r="B61" s="30" t="inlineStr">
         <is>
           <t xml:space="preserve">Certified that have personally checked the particulars of the Cadets mentioned above with reference to ser (a) to (l) and found them eligible in all respets to appear for Certificate "A" Exam 2018. </t>
         </is>
       </c>
     </row>
     <row r="62">
-      <c r="C62" s="46" t="inlineStr">
+      <c r="C62" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">SUMMARY </t>
         </is>
@@ -6257,7 +6257,7 @@
           <t xml:space="preserve">(a)  No. of  Cadets Eligible     :  </t>
         </is>
       </c>
-      <c r="E63" s="46" t="inlineStr">
+      <c r="E63" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Grading </t>
         </is>
@@ -6332,7 +6332,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="J69" s="52" t="inlineStr">
+      <c r="J69" s="29" t="inlineStr">
         <is>
           <t xml:space="preserve">Member's   : </t>
         </is>
@@ -6374,7 +6374,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="O77" s="52" t="n"/>
+      <c r="O77" s="29" t="n"/>
     </row>
     <row r="78">
       <c r="O78" s="27" t="inlineStr">
@@ -6406,39 +6406,6 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="O76:U76"/>
-    <mergeCell ref="O77:U77"/>
-    <mergeCell ref="O78:U78"/>
-    <mergeCell ref="O81:U81"/>
-    <mergeCell ref="O82:U82"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="O67:T67"/>
-    <mergeCell ref="J69:M69"/>
-    <mergeCell ref="O71:T71"/>
-    <mergeCell ref="O72:T72"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="O65:T65"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="O66:T66"/>
-    <mergeCell ref="B61:K61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="J63:O63"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="B12:Z12"/>
-    <mergeCell ref="Z8:Z9"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:U8"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="A1:Z1"/>
-    <mergeCell ref="A2:Z2"/>
-    <mergeCell ref="A3:Z3"/>
-    <mergeCell ref="A4:Z4"/>
-    <mergeCell ref="T5:Y5"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="T6:Y6"/>
     <mergeCell ref="A8:A10"/>
@@ -6455,6 +6422,39 @@
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="S9:U9"/>
     <mergeCell ref="G8:G10"/>
+    <mergeCell ref="A1:Z1"/>
+    <mergeCell ref="A2:Z2"/>
+    <mergeCell ref="A3:Z3"/>
+    <mergeCell ref="A4:Z4"/>
+    <mergeCell ref="T5:Y5"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="B12:Z12"/>
+    <mergeCell ref="Z8:Z9"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:U8"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="B61:K61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="J63:O63"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="O65:T65"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="O66:T66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="O67:T67"/>
+    <mergeCell ref="J69:M69"/>
+    <mergeCell ref="O71:T71"/>
+    <mergeCell ref="O72:T72"/>
+    <mergeCell ref="O76:U76"/>
+    <mergeCell ref="O77:U77"/>
+    <mergeCell ref="O78:U78"/>
+    <mergeCell ref="O81:U81"/>
+    <mergeCell ref="O82:U82"/>
   </mergeCells>
   <pageMargins left="1.25" right="0.7" top="0.5" bottom="1.01" header="0.3" footer="0.16"/>
   <pageSetup orientation="landscape" paperSize="5" scale="70" verticalDpi="0"/>

</xml_diff>